<commit_message>
Actualizacion de la Matriz de requisitos
</commit_message>
<xml_diff>
--- a/Documentacion/Matriz de requisitos Dacky.xlsx
+++ b/Documentacion/Matriz de requisitos Dacky.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicky\Documents\Proyecto Dacky\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyecto Dacky\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB6EB78-A71B-4B1E-A099-EF50DCD8DC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA84048A-822E-4733-B7BF-8306A8432928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="150">
   <si>
     <t>Fecha de la Versión:</t>
   </si>
@@ -347,308 +347,227 @@
     <t>X</t>
   </si>
   <si>
-    <t>Configurar zonas seguras (geocercas) y recibir alertas si la mascota las abandona</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>3.2</t>
-  </si>
-  <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>4.3</t>
-  </si>
-  <si>
-    <t>Crear, editar y ver perfiles de mascotas (nombre, raza, foto, fecha de nacimiento, etc.)</t>
-  </si>
-  <si>
-    <t>Registrar y actualizar información de vacunación (tipo de vacuna, fecha, próxima dosis)</t>
-  </si>
-  <si>
-    <t>Almacenar historial médico (alergias, enfermedades, cirugías)</t>
-  </si>
-  <si>
-    <t>Asociar el perfil de la mascota con el dispositivo de rastreo</t>
-  </si>
-  <si>
-    <t>Mostrar la ubicación actual de la mascota en un mapa</t>
-  </si>
-  <si>
-    <t>Permitir el seguimiento del historial de ubicaciones</t>
-  </si>
-  <si>
-    <t>Opción de activar el modo 'seguimiento en vivo' para actualizaciones más frecuentes</t>
-  </si>
-  <si>
-    <t>Generar un código QR único para cada mascota</t>
-  </si>
-  <si>
-    <t>Incluir en el código QR información de contacto del dueño (nombre, teléfono, correo electrónico)</t>
-  </si>
-  <si>
-    <t>Permitir que cualquier persona con un smartphone escanee el código y acceda a la información de contacto</t>
-  </si>
-  <si>
-    <t>Enviar notificaciones al dueño si la mascota abandona una zona segura</t>
-  </si>
-  <si>
-    <t>Notificar al dueño si la batería del dispositivo de rastreo está baja</t>
-  </si>
-  <si>
-    <t>Permitir al dueño enviar una notificación al dispositivo para que emita un sonido (útil si la mascota está cerca pero no visible)</t>
-  </si>
-  <si>
-    <t>Monitor de actividad física de la mascota (pasos, distancia recorrida)</t>
-  </si>
-  <si>
-    <t>Recordatorios de citas veterinarias y administración de medicamentos</t>
-  </si>
-  <si>
-    <t>Comunidad de usuarios para reportar mascotas perdidas o encontradas</t>
-  </si>
-  <si>
-    <t>Opción de recompensas por 'perdido'</t>
-  </si>
-  <si>
-    <t>Colaboración con guarderías locales, y paseos opcionales, paseos diarios (Personas encargadas)</t>
-  </si>
-  <si>
-    <t>Opción de llamada de emergencia, veterinaria y emergencia</t>
-  </si>
-  <si>
-    <t>Peluquería, ya domicilio, spa para mascotas</t>
-  </si>
-  <si>
-    <t>Entrenamiento canino</t>
-  </si>
-  <si>
-    <t>Productos para entrenamiento, accesorios, juguetes</t>
-  </si>
-  <si>
-    <t>Transporte canino (avión, bus, tren, etc.)</t>
-  </si>
-  <si>
-    <t>Suscrición con la app y especialistas</t>
-  </si>
-  <si>
-    <t>Colaboración con la app (transportación de vacunas y productos veterinarios)</t>
-  </si>
-  <si>
-    <t>Servicio funerario para mascotas</t>
-  </si>
-  <si>
-    <t>Seguro de mascotas</t>
-  </si>
-  <si>
-    <t>Servicio de cumpleaños</t>
-  </si>
-  <si>
-    <t>Opción de restaurante y comida para perros</t>
-  </si>
-  <si>
-    <t>Seguridad para mascotas, y rescates de animales (Rejas, guarda espaldas, cuidadores.)</t>
-  </si>
-  <si>
-    <t>Crear, editar y ver perfiles de mascotas</t>
-  </si>
-  <si>
     <t>Gestión de Hoja de Vida de Mascota</t>
   </si>
   <si>
     <t>Rastreo GPS en Tiempo Real</t>
   </si>
   <si>
-    <t>Código QR para Identificación y Contacto</t>
-  </si>
-  <si>
     <t>Notificaciones y Alertas</t>
-  </si>
-  <si>
-    <t>Registrar y actualizar información de vacunación</t>
-  </si>
-  <si>
-    <t>Almacenar historial médico</t>
-  </si>
-  <si>
-    <t>Configurar zonas seguras y recibir alertas</t>
-  </si>
-  <si>
-    <t>Opción de activar el modo 'seguimiento en vivo'</t>
-  </si>
-  <si>
-    <t>Incluir información de contacto del dueño en el código QR</t>
-  </si>
-  <si>
-    <t>Permitir que cualquier persona escanee el código y acceda a la información</t>
-  </si>
-  <si>
-    <t>Enviar notificaciones si la mascota abandona una zona segura</t>
-  </si>
-  <si>
-    <t>Notificar si la batería del dispositivo está baja</t>
-  </si>
-  <si>
-    <t>Permitir enviar una notificación para que el dispositivo emita un sonido</t>
-  </si>
-  <si>
-    <t>Funcionalidades Adicionales (Opcionales)</t>
-  </si>
-  <si>
-    <t>Monitor de actividad física de la mascota</t>
-  </si>
-  <si>
-    <t>Colaboración con guarderías locales y paseos opcionales</t>
-  </si>
-  <si>
-    <t>Opción de llamada de emergencia</t>
-  </si>
-  <si>
-    <t>Peluquería</t>
-  </si>
-  <si>
-    <t>Productos para entrenamiento</t>
-  </si>
-  <si>
-    <t>Transporte canino</t>
-  </si>
-  <si>
-    <t>Colaboración con la app</t>
-  </si>
-  <si>
-    <t>Seguridad para mascotas</t>
-  </si>
-  <si>
-    <t>5.1</t>
-  </si>
-  <si>
-    <t>5.2</t>
-  </si>
-  <si>
-    <t>5.3</t>
-  </si>
-  <si>
-    <t>5.4</t>
-  </si>
-  <si>
-    <t>5.5</t>
-  </si>
-  <si>
-    <t>5.6</t>
-  </si>
-  <si>
-    <t>5.7</t>
-  </si>
-  <si>
-    <t>5.8</t>
-  </si>
-  <si>
-    <t>5.9</t>
-  </si>
-  <si>
-    <t>5.10</t>
-  </si>
-  <si>
-    <t>5.11</t>
-  </si>
-  <si>
-    <t>5.12</t>
-  </si>
-  <si>
-    <t>5.13</t>
-  </si>
-  <si>
-    <t>5.14</t>
-  </si>
-  <si>
-    <t>5.15</t>
-  </si>
-  <si>
-    <t>5.16</t>
-  </si>
-  <si>
-    <t>5.17</t>
   </si>
   <si>
     <t>Descripcion</t>
   </si>
   <si>
-    <t>Cada perro registrado en la aplicación debe tener una "Hoja de vida" que incluya datos básicos como nombre, raza, edad, y dueño.</t>
+    <t>Creación de perfil</t>
   </si>
   <si>
-    <t>La tarjeta virtual de vacunas debe estar actualizada y ser accesible en cualquier momento desde la aplicación.</t>
+    <t>Edición y eliminación de perfil</t>
   </si>
   <si>
-    <t>El GPS debe estar activo en todo momento, permitiendo a los usuarios rastrear la ubicación de su perro en tiempo real.</t>
+    <t>Solo el usuario registrado podrá modificar la información de su mascota</t>
   </si>
   <si>
-    <t>El código QR en el collar del perro debe redirigir automáticamente a la página de contacto del dueño cuando es escaneado.</t>
+    <t>Localización en tiempo real</t>
   </si>
   <si>
-    <t>Solo usuarios autenticados pueden modificar la información del perro o acceder al historial de ubicación.</t>
+    <t>Historial de ubicaciones</t>
   </si>
   <si>
-    <t>En caso de que un perro se extravíe, el dueño debe recibir una notificación inmediata con la última ubicación registrada.</t>
+    <t>Registro de vacunas</t>
   </si>
   <si>
-    <t>La aplicación debe cumplir con todas las normativas de protección de datos vigentes en la región de uso.</t>
+    <t>El sistema generará alertas cuando se acerque la fecha de una nueva vacuna.</t>
   </si>
   <si>
-    <t>Información básica del perro: nombre, raza, edad, peso, color, y una foto reciente.</t>
+    <t>Consulta del historial de vacunas</t>
   </si>
   <si>
-    <t>Datos de contacto del dueño: nombre completo, número de teléfono, dirección de correo electrónico.</t>
+    <t xml:space="preserve"> Tarjeta de Vacunas Virtual</t>
   </si>
   <si>
-    <t>Historial de vacunación del perro: fecha, tipo de vacuna, y veterinario responsable.</t>
+    <t>Acceso a información de la mascota</t>
   </si>
   <si>
-    <t>Información del dispositivo GPS: número de serie, estado de la batería, y última ubicación conocida.</t>
+    <t>Opciones de contacto</t>
   </si>
   <si>
-    <t>Registro de eventos de rastreo: fecha, hora, y coordenadas de cada actualización de ubicación.</t>
+    <t>Escaneo de QR</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
+    <t>Alertas por salida de zona segura</t>
+  </si>
+  <si>
+    <t>Alertas de actividad de la mascota</t>
+  </si>
+  <si>
+    <t>Se podrán agendar servicios de peluquería, spa para mascotas y atención a domicilio.</t>
+  </si>
+  <si>
+    <t>La app ofrecerá acceso a entrenamientos caninos y productos de entrenamiento, como accesorios y juguetes.</t>
+  </si>
+  <si>
+    <t>Se proporcionará un servicio de transporte para mascotas por avión, bus o tren.</t>
+  </si>
+  <si>
+    <t>Se habilitará una suscripción con la app y especialistas en bienestar animal.</t>
+  </si>
+  <si>
+    <t>Habrá una colaboración con empresas para el transporte de vacunas y productos veterinarios.</t>
+  </si>
+  <si>
+    <t>Se integrará un servicio funerario para mascotas.</t>
+  </si>
+  <si>
+    <t>Se incluirá un seguro de mascotas para cubrir emergencias y tratamientos médicos.</t>
+  </si>
+  <si>
+    <t>La app ofrecerá la posibilidad de organizar eventos de cumpleaños para mascotas.</t>
+  </si>
+  <si>
+    <t>Se habilitará una opción de búsqueda de restaurantes y comida especializada para mascotas.</t>
+  </si>
+  <si>
+    <t>Se brindará un módulo de seguridad para mascotas, incluyendo rescates, rejas de protección y cuidadores especializados.</t>
+  </si>
+  <si>
+    <t>El usuario podrá registrar una nueva mascota ingresando nombre, raza, edad y foto</t>
+  </si>
+  <si>
+    <t>El usuario podrá adjuntar información médica relevante</t>
+  </si>
+  <si>
+    <t>El sistema validará que todos los campos obligatorios estén completos antes de guardar el perfil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  El usuario podrá modificar los datos de su mascota en cualquier momento</t>
+  </si>
+  <si>
+    <t>Solo el usuario propietario podrá eliminar el perfil de su mascota</t>
+  </si>
+  <si>
+    <t>El sistema no permitirá eliminar un perfil si está vinculado a un rastreador activo</t>
+  </si>
+  <si>
+    <t>El usuario podrá visualizar la ubicación de su mascota en un mapa interactivo</t>
+  </si>
+  <si>
+    <t>El sistema actualizará la ubicación cada X segundos según la configuración establecida</t>
+  </si>
+  <si>
+    <t>La precisión de la ubicación dependerá de la señal GPS y la conectividad del collar</t>
+  </si>
+  <si>
+    <t>El usuario podrá consultar las ubicaciones registradas en un período de tiempo determinado</t>
+  </si>
+  <si>
+    <t>El sistema mostrará un recorrido de los movimientos de la mascota</t>
+  </si>
+  <si>
+    <t>Se podrán generar reportes del historial de ubicación</t>
+  </si>
+  <si>
+    <t>El usuario podrá registrar las vacunas administradas a su mascota</t>
+  </si>
+  <si>
+    <t>Se podrá adjuntar la fecha de aplicación y el veterinario responsable</t>
+  </si>
+  <si>
+    <t>El sistema generará alertas cuando se acerque la fecha de una nueva vacuna</t>
+  </si>
+  <si>
+    <t>El usuario podrá visualizar todas las vacunas registradas</t>
+  </si>
+  <si>
+    <t>Se podrán exportar los datos en un documento PDF</t>
+  </si>
+  <si>
+    <t>Cualquier persona podrá escanear el código QR del collar para acceder a información básica de la mascota</t>
+  </si>
+  <si>
+    <t>Se mostrará el nombre de la mascota y los datos de contacto del dueño si este lo permite</t>
+  </si>
+  <si>
+    <t>La persona que escanea el QR podrá contactar al dueño mediante llamada o mensaje</t>
+  </si>
+  <si>
+    <t>El sistema enviará una notificación al dueño cuando su mascota sea escaneada</t>
+  </si>
+  <si>
+    <t>El usuario podrá definir un área segura para su mascota</t>
+  </si>
+  <si>
+    <t>El sistema enviará una notificación si la mascota sale del área definida</t>
+  </si>
+  <si>
+    <t>Se enviarán alertas si la mascota se encuentra inactiva durante un período prolongado</t>
+  </si>
+  <si>
+    <t>Se notificará al usuario cuando el collar tenga batería baja</t>
+  </si>
+  <si>
+    <t>El sistema permitirá a los usuarios acceder a un monitor de actividad física de su mascota, incluyendo pasos y distancia recorrida</t>
+  </si>
+  <si>
+    <t>Se ofrecerán recordatorios de citas veterinarias y administración de medicamentos</t>
+  </si>
+  <si>
+    <t>La app incluirá una comunidad de usuarios para reportar mascotas perdidas o encontradas</t>
+  </si>
+  <si>
+    <t>Existirá una opción de recompensas por mascotas perdidas para incentivar su recuperación</t>
+  </si>
+  <si>
+    <t>Se colaborará con guarderías locales y paseadores de mascotas para ofrecer paseos diarios y cuidados personalizados</t>
+  </si>
+  <si>
+    <t>Se incluirá una opción de llamada de emergencia tanto a veterinarias como a servicios de urgencia</t>
+  </si>
+  <si>
+    <t>Servicios Adicionales (No aplican para la version BETA)</t>
+  </si>
+  <si>
+    <t>No se puede eliminar un perfil si está vinculado a un rastreador activo.</t>
+  </si>
+  <si>
+    <t>Solo el dueño de la mascota puede acceder a la ubicación en tiempo real.</t>
+  </si>
+  <si>
+    <t>El sistema debe actualizar la ubicación cada cierto tiempo.</t>
+  </si>
+  <si>
+    <t>Solo los usuarios con permisos pueden modificar el registro de vacunas.</t>
+  </si>
+  <si>
+    <t>No se pueden registrar fechas de vacunación futuras.</t>
+  </si>
+  <si>
+    <t>Solo se mostrará la información autorizada por el dueño.</t>
+  </si>
+  <si>
+    <t>No se podrá modificar la información desde el acceso QR.</t>
+  </si>
+  <si>
+    <t>El usuario debe haber definido un área segura previamente</t>
+  </si>
+  <si>
+    <t>Las alertas solo se enviarán si el rastreo GPS está activo.</t>
+  </si>
+  <si>
+    <t>Se aplicaran estos servicios adicionales a traves de actualizaciones</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>Funcionalidades Adicionales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -753,17 +672,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -776,8 +684,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -850,8 +784,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1239,11 +1179,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1340,43 +1317,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1388,50 +1332,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1445,22 +1353,10 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1472,32 +1368,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1506,11 +1376,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1545,6 +1426,117 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1553,6 +1545,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFFFCCCC"/>
     </mruColors>
   </colors>
@@ -1767,18 +1760,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="67" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
-    <col min="4" max="4" width="123" customWidth="1"/>
+    <col min="4" max="4" width="135.42578125" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="60.5703125" customWidth="1"/>
+    <col min="6" max="6" width="74.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="44.85546875" customWidth="1"/>
     <col min="9" max="11" width="88.7109375" customWidth="1"/>
@@ -1825,7 +1818,7 @@
       <c r="AA3" s="4"/>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="57" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="8"/>
@@ -1856,20 +1849,20 @@
       <c r="AA4" s="4"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1">
-      <c r="A5" s="75"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="85" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="87" t="s">
+      <c r="D5" s="59"/>
+      <c r="E5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="88"/>
-      <c r="G5" s="87" t="s">
+      <c r="F5" s="61"/>
+      <c r="G5" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="89"/>
+      <c r="H5" s="62"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -1891,28 +1884,28 @@
       <c r="AA5" s="10"/>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="79" t="s">
-        <v>163</v>
+      <c r="D6" s="120" t="s">
+        <v>81</v>
       </c>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="82" t="s">
+      <c r="G6" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="77" t="s">
+      <c r="H6" s="54" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="11"/>
@@ -1935,31 +1928,23 @@
       <c r="Z6" s="11"/>
       <c r="AA6" s="11"/>
     </row>
-    <row r="7" spans="1:27" ht="45" customHeight="1">
-      <c r="A7" s="90" t="s">
-        <v>124</v>
+    <row r="7" spans="1:27" ht="18.75" customHeight="1">
+      <c r="A7" s="106" t="s">
+        <v>78</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>123</v>
+      <c r="B7" s="105" t="s">
+        <v>82</v>
       </c>
-      <c r="C7" s="67" t="s">
-        <v>79</v>
+      <c r="C7" s="97"/>
+      <c r="D7" s="95" t="s">
+        <v>106</v>
       </c>
-      <c r="D7" s="51" t="s">
-        <v>93</v>
+      <c r="E7" s="97"/>
+      <c r="F7" s="95" t="s">
+        <v>84</v>
       </c>
-      <c r="E7" s="70">
-        <v>1</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="G7" s="62">
-        <v>1</v>
-      </c>
-      <c r="H7" s="50" t="s">
-        <v>171</v>
-      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="45"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -1980,29 +1965,19 @@
       <c r="Z7" s="11"/>
       <c r="AA7" s="11"/>
     </row>
-    <row r="8" spans="1:27" ht="30" customHeight="1">
-      <c r="A8" s="91"/>
-      <c r="B8" s="51" t="s">
-        <v>128</v>
+    <row r="8" spans="1:27" ht="18" customHeight="1">
+      <c r="A8" s="106"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="95" t="s">
+        <v>107</v>
       </c>
-      <c r="C8" s="67" t="s">
-        <v>80</v>
+      <c r="E8" s="97"/>
+      <c r="F8" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="D8" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="71">
-        <v>2</v>
-      </c>
-      <c r="F8" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="G8" s="63">
-        <v>2</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>172</v>
-      </c>
+      <c r="G8" s="49"/>
+      <c r="H8" s="45"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -2023,29 +1998,19 @@
       <c r="Z8" s="11"/>
       <c r="AA8" s="11"/>
     </row>
-    <row r="9" spans="1:27" ht="30" customHeight="1">
-      <c r="A9" s="91"/>
-      <c r="B9" s="51" t="s">
-        <v>129</v>
+    <row r="9" spans="1:27" ht="16.5" customHeight="1">
+      <c r="A9" s="106"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="95" t="s">
+        <v>108</v>
       </c>
-      <c r="C9" s="67" t="s">
-        <v>81</v>
+      <c r="E9" s="97"/>
+      <c r="F9" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="D9" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="70">
-        <v>3</v>
-      </c>
-      <c r="F9" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="G9" s="62">
-        <v>3</v>
-      </c>
-      <c r="H9" s="50" t="s">
-        <v>173</v>
-      </c>
+      <c r="G9" s="49"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
@@ -2066,29 +2031,15 @@
       <c r="Z9" s="11"/>
       <c r="AA9" s="11"/>
     </row>
-    <row r="10" spans="1:27" ht="45">
-      <c r="A10" s="91"/>
-      <c r="B10" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="70">
-        <v>4</v>
-      </c>
-      <c r="F10" s="60" t="s">
-        <v>167</v>
-      </c>
-      <c r="G10" s="62">
-        <v>4</v>
-      </c>
-      <c r="H10" s="50" t="s">
-        <v>174</v>
-      </c>
+    <row r="10" spans="1:27" ht="20.25" customHeight="1">
+      <c r="A10" s="106"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="45"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -2109,25 +2060,21 @@
       <c r="Z10" s="11"/>
       <c r="AA10" s="11"/>
     </row>
-    <row r="11" spans="1:27" ht="45">
-      <c r="A11" s="91"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="46" t="s">
-        <v>176</v>
+    <row r="11" spans="1:27" ht="15.75">
+      <c r="A11" s="106"/>
+      <c r="B11" s="105" t="s">
+        <v>83</v>
       </c>
-      <c r="E11" s="70">
-        <v>5</v>
+      <c r="C11" s="97"/>
+      <c r="D11" s="104" t="s">
+        <v>109</v>
       </c>
-      <c r="F11" s="50" t="s">
-        <v>168</v>
+      <c r="E11" s="97"/>
+      <c r="F11" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="G11" s="62">
-        <v>5</v>
-      </c>
-      <c r="H11" s="50" t="s">
-        <v>174</v>
-      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="45"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
@@ -2148,23 +2095,19 @@
       <c r="Z11" s="11"/>
       <c r="AA11" s="11"/>
     </row>
-    <row r="12" spans="1:27" ht="28.5" customHeight="1">
-      <c r="A12" s="91"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="70">
-        <v>6</v>
+    <row r="12" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A12" s="106"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="95" t="s">
+        <v>110</v>
       </c>
-      <c r="F12" s="50" t="s">
-        <v>169</v>
+      <c r="E12" s="97"/>
+      <c r="F12" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="G12" s="62">
-        <v>6</v>
-      </c>
-      <c r="H12" s="50" t="s">
-        <v>175</v>
-      </c>
+      <c r="G12" s="49"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
@@ -2185,23 +2128,19 @@
       <c r="Z12" s="11"/>
       <c r="AA12" s="11"/>
     </row>
-    <row r="13" spans="1:27" ht="28.5" customHeight="1">
-      <c r="A13" s="91"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="71">
-        <v>7</v>
+    <row r="13" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A13" s="106"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="95" t="s">
+        <v>111</v>
       </c>
-      <c r="F13" s="48" t="s">
-        <v>170</v>
+      <c r="E13" s="97"/>
+      <c r="F13" s="107" t="s">
+        <v>138</v>
       </c>
-      <c r="G13" s="63">
-        <v>7</v>
-      </c>
-      <c r="H13" s="50" t="s">
-        <v>175</v>
-      </c>
+      <c r="G13" s="49"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
@@ -2223,14 +2162,14 @@
       <c r="AA13" s="11"/>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A14" s="91"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="50"/>
+      <c r="A14" s="123"/>
+      <c r="B14" s="123"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
@@ -2252,14 +2191,22 @@
       <c r="AA14" s="11"/>
     </row>
     <row r="15" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A15" s="91"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="66"/>
+      <c r="A15" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="96"/>
+      <c r="D15" s="107" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="96"/>
+      <c r="F15" s="107" t="s">
+        <v>139</v>
+      </c>
+      <c r="G15" s="49"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -2281,14 +2228,18 @@
       <c r="AA15" s="11"/>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A16" s="92"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="66"/>
+      <c r="A16" s="106"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="97"/>
+      <c r="F16" s="104" t="s">
+        <v>148</v>
+      </c>
+      <c r="G16" s="49"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -2310,22 +2261,18 @@
       <c r="AA16" s="11"/>
     </row>
     <row r="17" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A17" s="90" t="s">
-        <v>125</v>
+      <c r="A17" s="106"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="95" t="s">
+        <v>114</v>
       </c>
-      <c r="B17" s="51" t="s">
-        <v>97</v>
+      <c r="E17" s="110"/>
+      <c r="F17" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="C17" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="72"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="66"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
@@ -2347,20 +2294,14 @@
       <c r="AA17" s="11"/>
     </row>
     <row r="18" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A18" s="91"/>
-      <c r="B18" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="66"/>
+      <c r="A18" s="106"/>
+      <c r="B18" s="100"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="50"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
@@ -2382,20 +2323,20 @@
       <c r="AA18" s="11"/>
     </row>
     <row r="19" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A19" s="91"/>
-      <c r="B19" s="51" t="s">
-        <v>130</v>
+      <c r="A19" s="106"/>
+      <c r="B19" s="105" t="s">
+        <v>86</v>
       </c>
-      <c r="C19" s="67" t="s">
-        <v>85</v>
+      <c r="C19" s="97"/>
+      <c r="D19" s="95" t="s">
+        <v>115</v>
       </c>
-      <c r="D19" s="51" t="s">
-        <v>78</v>
+      <c r="E19" s="110"/>
+      <c r="F19" s="107" t="s">
+        <v>140</v>
       </c>
-      <c r="E19" s="72"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="66"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="50"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
@@ -2417,20 +2358,18 @@
       <c r="AA19" s="11"/>
     </row>
     <row r="20" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A20" s="91"/>
-      <c r="B20" s="51" t="s">
-        <v>131</v>
+      <c r="A20" s="106"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="95" t="s">
+        <v>116</v>
       </c>
-      <c r="C20" s="67" t="s">
-        <v>86</v>
+      <c r="E20" s="110"/>
+      <c r="F20" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="D20" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="72"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="66"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
@@ -2452,14 +2391,18 @@
       <c r="AA20" s="11"/>
     </row>
     <row r="21" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A21" s="91"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="66"/>
+      <c r="A21" s="106"/>
+      <c r="B21" s="105"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="110"/>
+      <c r="F21" s="104" t="s">
+        <v>148</v>
+      </c>
+      <c r="G21" s="101"/>
+      <c r="H21" s="50"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
@@ -2481,14 +2424,14 @@
       <c r="AA21" s="11"/>
     </row>
     <row r="22" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A22" s="91"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="66"/>
+      <c r="A22" s="106"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="101"/>
+      <c r="H22" s="50"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
@@ -2510,14 +2453,22 @@
       <c r="AA22" s="11"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="91"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="66"/>
+      <c r="A23" s="106" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="105" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="97"/>
+      <c r="D23" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="110"/>
+      <c r="F23" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="101"/>
+      <c r="H23" s="50"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
@@ -2539,14 +2490,18 @@
       <c r="AA23" s="11"/>
     </row>
     <row r="24" spans="1:27" ht="15" customHeight="1">
-      <c r="A24" s="91"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="66"/>
+      <c r="A24" s="106"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="107" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="110"/>
+      <c r="F24" s="107" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="101"/>
+      <c r="H24" s="50"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
@@ -2568,14 +2523,18 @@
       <c r="AA24" s="11"/>
     </row>
     <row r="25" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A25" s="91"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="66"/>
+      <c r="A25" s="106"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="107" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="110"/>
+      <c r="F25" s="104" t="s">
+        <v>148</v>
+      </c>
+      <c r="G25" s="101"/>
+      <c r="H25" s="50"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
@@ -2597,14 +2556,14 @@
       <c r="AA25" s="11"/>
     </row>
     <row r="26" spans="1:27" ht="14.25" hidden="1" customHeight="1">
-      <c r="A26" s="91"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="66"/>
+      <c r="A26" s="106"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="97"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="101"/>
+      <c r="H26" s="50"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
@@ -2626,14 +2585,16 @@
       <c r="AA26" s="11"/>
     </row>
     <row r="27" spans="1:27" ht="14.25" hidden="1" customHeight="1">
-      <c r="A27" s="91"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="66"/>
+      <c r="A27" s="106"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="107" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="110"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="101"/>
+      <c r="H27" s="50"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
@@ -2655,14 +2616,14 @@
       <c r="AA27" s="11"/>
     </row>
     <row r="28" spans="1:27" ht="14.25" hidden="1" customHeight="1">
-      <c r="A28" s="91"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="66"/>
+      <c r="A28" s="106"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="50"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
@@ -2684,14 +2645,14 @@
       <c r="AA28" s="11"/>
     </row>
     <row r="29" spans="1:27" ht="14.25" hidden="1" customHeight="1">
-      <c r="A29" s="91"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="66"/>
+      <c r="A29" s="106"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="50"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
@@ -2713,14 +2674,14 @@
       <c r="AA29" s="11"/>
     </row>
     <row r="30" spans="1:27" ht="14.25" hidden="1" customHeight="1">
-      <c r="A30" s="91"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="66"/>
+      <c r="A30" s="106"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="101"/>
+      <c r="H30" s="50"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
@@ -2742,14 +2703,14 @@
       <c r="AA30" s="11"/>
     </row>
     <row r="31" spans="1:27" ht="14.25" hidden="1" customHeight="1">
-      <c r="A31" s="91"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="66"/>
+      <c r="A31" s="106"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="108"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="50"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
@@ -2771,14 +2732,14 @@
       <c r="AA31" s="11"/>
     </row>
     <row r="32" spans="1:27" ht="14.25" hidden="1" customHeight="1">
-      <c r="A32" s="91"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="66"/>
+      <c r="A32" s="106"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="108"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="50"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
@@ -2800,14 +2761,14 @@
       <c r="AA32" s="11"/>
     </row>
     <row r="33" spans="1:27" ht="14.25" hidden="1" customHeight="1">
-      <c r="A33" s="92"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="66"/>
+      <c r="A33" s="106"/>
+      <c r="B33" s="96"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="108"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="50"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
@@ -2829,22 +2790,14 @@
       <c r="AA33" s="11"/>
     </row>
     <row r="34" spans="1:27" ht="15" customHeight="1">
-      <c r="A34" s="90" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="67" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="73"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="66"/>
+      <c r="A34" s="106"/>
+      <c r="B34" s="100"/>
+      <c r="C34" s="100"/>
+      <c r="D34" s="100"/>
+      <c r="E34" s="100"/>
+      <c r="F34" s="100"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="50"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -2866,20 +2819,20 @@
       <c r="AA34" s="4"/>
     </row>
     <row r="35" spans="1:27" ht="15" customHeight="1">
-      <c r="A35" s="91"/>
-      <c r="B35" s="51" t="s">
-        <v>132</v>
+      <c r="A35" s="106"/>
+      <c r="B35" s="105" t="s">
+        <v>89</v>
       </c>
-      <c r="C35" s="67" t="s">
-        <v>88</v>
+      <c r="C35" s="97"/>
+      <c r="D35" s="95" t="s">
+        <v>121</v>
       </c>
-      <c r="D35" s="51" t="s">
-        <v>101</v>
+      <c r="E35" s="111"/>
+      <c r="F35" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="E35" s="73"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="66"/>
+      <c r="G35" s="102"/>
+      <c r="H35" s="50"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -2901,20 +2854,18 @@
       <c r="AA35" s="4"/>
     </row>
     <row r="36" spans="1:27" ht="15" customHeight="1">
-      <c r="A36" s="91"/>
-      <c r="B36" s="51" t="s">
-        <v>133</v>
+      <c r="A36" s="106"/>
+      <c r="B36" s="105"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="95" t="s">
+        <v>122</v>
       </c>
-      <c r="C36" s="67" t="s">
-        <v>89</v>
+      <c r="E36" s="111"/>
+      <c r="F36" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="D36" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="E36" s="73"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="66"/>
+      <c r="G36" s="102"/>
+      <c r="H36" s="50"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2936,14 +2887,14 @@
       <c r="AA36" s="4"/>
     </row>
     <row r="37" spans="1:27" ht="15" customHeight="1">
-      <c r="A37" s="91"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="66"/>
+      <c r="A37" s="106"/>
+      <c r="B37" s="106"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="106"/>
+      <c r="G37" s="102"/>
+      <c r="H37" s="50"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -2965,14 +2916,22 @@
       <c r="AA37" s="4"/>
     </row>
     <row r="38" spans="1:27" ht="15" customHeight="1">
-      <c r="A38" s="91"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="66"/>
+      <c r="A38" s="109" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="97"/>
+      <c r="D38" s="95" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" s="111"/>
+      <c r="F38" s="107" t="s">
+        <v>143</v>
+      </c>
+      <c r="G38" s="102"/>
+      <c r="H38" s="50"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -2994,14 +2953,18 @@
       <c r="AA38" s="4"/>
     </row>
     <row r="39" spans="1:27" ht="15" customHeight="1">
-      <c r="A39" s="92"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="66"/>
+      <c r="A39" s="109"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="95" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" s="111"/>
+      <c r="F39" s="104" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="102"/>
+      <c r="H39" s="50"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3023,22 +2986,14 @@
       <c r="AA39" s="4"/>
     </row>
     <row r="40" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A40" s="90" t="s">
-        <v>127</v>
-      </c>
-      <c r="B40" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="C40" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="51" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="73"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="66"/>
+      <c r="A40" s="109"/>
+      <c r="B40" s="105"/>
+      <c r="C40" s="105"/>
+      <c r="D40" s="105"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="105"/>
+      <c r="G40" s="103"/>
+      <c r="H40" s="50"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -3060,20 +3015,20 @@
       <c r="AA40" s="4"/>
     </row>
     <row r="41" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A41" s="91"/>
-      <c r="B41" s="51" t="s">
-        <v>135</v>
+      <c r="A41" s="109"/>
+      <c r="B41" s="105" t="s">
+        <v>92</v>
       </c>
-      <c r="C41" s="67" t="s">
-        <v>91</v>
+      <c r="C41" s="97"/>
+      <c r="D41" s="95" t="s">
+        <v>125</v>
       </c>
-      <c r="D41" s="51" t="s">
-        <v>104</v>
+      <c r="E41" s="111"/>
+      <c r="F41" s="107" t="s">
+        <v>144</v>
       </c>
-      <c r="E41" s="73"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="66"/>
+      <c r="G41" s="103"/>
+      <c r="H41" s="50"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -3095,20 +3050,18 @@
       <c r="AA41" s="4"/>
     </row>
     <row r="42" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A42" s="91"/>
-      <c r="B42" s="51" t="s">
-        <v>136</v>
+      <c r="A42" s="109"/>
+      <c r="B42" s="105"/>
+      <c r="C42" s="97"/>
+      <c r="D42" s="95" t="s">
+        <v>126</v>
       </c>
-      <c r="C42" s="67" t="s">
-        <v>92</v>
+      <c r="E42" s="111"/>
+      <c r="F42" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="D42" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="E42" s="73"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="66"/>
+      <c r="G42" s="103"/>
+      <c r="H42" s="50"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -3130,14 +3083,14 @@
       <c r="AA42" s="4"/>
     </row>
     <row r="43" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A43" s="91"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="67"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="66"/>
+      <c r="A43" s="109"/>
+      <c r="B43" s="109"/>
+      <c r="C43" s="109"/>
+      <c r="D43" s="109"/>
+      <c r="E43" s="109"/>
+      <c r="F43" s="109"/>
+      <c r="G43" s="103"/>
+      <c r="H43" s="113"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -3159,16 +3112,24 @@
       <c r="AA43" s="4"/>
     </row>
     <row r="44" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A44" s="91"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="67"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
+      <c r="A44" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="105" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="96"/>
+      <c r="D44" s="95" t="s">
+        <v>127</v>
+      </c>
+      <c r="E44" s="96"/>
+      <c r="F44" s="107" t="s">
+        <v>145</v>
+      </c>
+      <c r="G44" s="117"/>
+      <c r="H44" s="96"/>
+      <c r="I44" s="116"/>
+      <c r="J44" s="116"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
@@ -3188,14 +3149,18 @@
       <c r="AA44" s="4"/>
     </row>
     <row r="45" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A45" s="91"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="67"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="66"/>
+      <c r="A45" s="106"/>
+      <c r="B45" s="105"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="95" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="96"/>
+      <c r="F45" s="104" t="s">
+        <v>148</v>
+      </c>
+      <c r="G45" s="103"/>
+      <c r="H45" s="118"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -3217,14 +3182,14 @@
       <c r="AA45" s="4"/>
     </row>
     <row r="46" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A46" s="91"/>
-      <c r="B46" s="53"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="66"/>
+      <c r="A46" s="106"/>
+      <c r="B46" s="99"/>
+      <c r="C46" s="99"/>
+      <c r="D46" s="99"/>
+      <c r="E46" s="99"/>
+      <c r="F46" s="99"/>
+      <c r="G46" s="103"/>
+      <c r="H46" s="50"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -3246,22 +3211,20 @@
       <c r="AA46" s="4"/>
     </row>
     <row r="47" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A47" s="84" t="s">
-        <v>137</v>
+      <c r="A47" s="106"/>
+      <c r="B47" s="105" t="s">
+        <v>95</v>
       </c>
-      <c r="B47" s="51" t="s">
-        <v>138</v>
+      <c r="C47" s="97"/>
+      <c r="D47" s="95" t="s">
+        <v>129</v>
       </c>
-      <c r="C47" s="67" t="s">
+      <c r="E47" s="111"/>
+      <c r="F47" s="107" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="E47" s="73"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="66"/>
+      <c r="G47" s="103"/>
+      <c r="H47" s="50"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -3283,20 +3246,18 @@
       <c r="AA47" s="4"/>
     </row>
     <row r="48" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A48" s="84"/>
-      <c r="B48" s="51" t="s">
-        <v>107</v>
+      <c r="A48" s="106"/>
+      <c r="B48" s="105"/>
+      <c r="C48" s="97"/>
+      <c r="D48" s="95" t="s">
+        <v>130</v>
       </c>
-      <c r="C48" s="67" t="s">
-        <v>147</v>
+      <c r="E48" s="111"/>
+      <c r="F48" s="104" t="s">
+        <v>148</v>
       </c>
-      <c r="D48" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48" s="73"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="66"/>
+      <c r="G48" s="103"/>
+      <c r="H48" s="50"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -3318,20 +3279,14 @@
       <c r="AA48" s="4"/>
     </row>
     <row r="49" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A49" s="84"/>
-      <c r="B49" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="D49" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="E49" s="73"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="66"/>
+      <c r="A49" s="124"/>
+      <c r="B49" s="124"/>
+      <c r="C49" s="124"/>
+      <c r="D49" s="124"/>
+      <c r="E49" s="124"/>
+      <c r="F49" s="124"/>
+      <c r="G49" s="103"/>
+      <c r="H49" s="50"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -3352,21 +3307,23 @@
       <c r="Z49" s="4"/>
       <c r="AA49" s="4"/>
     </row>
-    <row r="50" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A50" s="84"/>
-      <c r="B50" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="C50" s="67" t="s">
+    <row r="50" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A50" s="127" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="51" t="s">
-        <v>109</v>
+      <c r="B50" s="128" t="s">
+        <v>137</v>
       </c>
-      <c r="E50" s="73"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="66"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="119" t="s">
+        <v>131</v>
+      </c>
+      <c r="E50" s="129"/>
+      <c r="F50" s="104" t="s">
+        <v>147</v>
+      </c>
+      <c r="G50" s="103"/>
+      <c r="H50" s="50"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -3387,21 +3344,19 @@
       <c r="Z50" s="4"/>
       <c r="AA50" s="4"/>
     </row>
-    <row r="51" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A51" s="84"/>
-      <c r="B51" s="51" t="s">
-        <v>139</v>
+    <row r="51" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A51" s="127"/>
+      <c r="B51" s="128"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="119" t="s">
+        <v>132</v>
       </c>
-      <c r="C51" s="67" t="s">
-        <v>150</v>
+      <c r="E51" s="129"/>
+      <c r="F51" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D51" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="E51" s="73"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="66"/>
+      <c r="G51" s="103"/>
+      <c r="H51" s="50"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -3422,21 +3377,19 @@
       <c r="Z51" s="4"/>
       <c r="AA51" s="4"/>
     </row>
-    <row r="52" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A52" s="84"/>
-      <c r="B52" s="51" t="s">
-        <v>140</v>
+    <row r="52" spans="1:27" ht="18" customHeight="1">
+      <c r="A52" s="127"/>
+      <c r="B52" s="128"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="119" t="s">
+        <v>133</v>
       </c>
-      <c r="C52" s="67" t="s">
-        <v>151</v>
+      <c r="E52" s="129"/>
+      <c r="F52" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D52" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" s="73"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="61"/>
-      <c r="H52" s="66"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="50"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -3457,21 +3410,19 @@
       <c r="Z52" s="4"/>
       <c r="AA52" s="4"/>
     </row>
-    <row r="53" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A53" s="84"/>
-      <c r="B53" s="51" t="s">
-        <v>141</v>
+    <row r="53" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A53" s="127"/>
+      <c r="B53" s="128"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="119" t="s">
+        <v>134</v>
       </c>
-      <c r="C53" s="67" t="s">
-        <v>152</v>
+      <c r="E53" s="129"/>
+      <c r="F53" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D53" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="E53" s="73"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="61"/>
-      <c r="H53" s="66"/>
+      <c r="G53" s="103"/>
+      <c r="H53" s="50"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -3492,21 +3443,19 @@
       <c r="Z53" s="4"/>
       <c r="AA53" s="4"/>
     </row>
-    <row r="54" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A54" s="84"/>
-      <c r="B54" s="51" t="s">
-        <v>113</v>
+    <row r="54" spans="1:27" ht="16.5" customHeight="1">
+      <c r="A54" s="127"/>
+      <c r="B54" s="128"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="119" t="s">
+        <v>135</v>
       </c>
-      <c r="C54" s="67" t="s">
-        <v>153</v>
+      <c r="E54" s="129"/>
+      <c r="F54" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D54" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="E54" s="73"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="61"/>
-      <c r="H54" s="66"/>
+      <c r="G54" s="103"/>
+      <c r="H54" s="50"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -3527,21 +3476,19 @@
       <c r="Z54" s="4"/>
       <c r="AA54" s="4"/>
     </row>
-    <row r="55" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A55" s="84"/>
-      <c r="B55" s="51" t="s">
-        <v>142</v>
+    <row r="55" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A55" s="127"/>
+      <c r="B55" s="128"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="119" t="s">
+        <v>136</v>
       </c>
-      <c r="C55" s="67" t="s">
-        <v>154</v>
+      <c r="E55" s="129"/>
+      <c r="F55" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D55" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E55" s="73"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="61"/>
-      <c r="H55" s="66"/>
+      <c r="G55" s="103"/>
+      <c r="H55" s="50"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -3562,21 +3509,19 @@
       <c r="Z55" s="4"/>
       <c r="AA55" s="4"/>
     </row>
-    <row r="56" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A56" s="84"/>
-      <c r="B56" s="51" t="s">
-        <v>143</v>
+    <row r="56" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A56" s="127"/>
+      <c r="B56" s="128"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="119" t="s">
+        <v>96</v>
       </c>
-      <c r="C56" s="67" t="s">
-        <v>155</v>
+      <c r="E56" s="129"/>
+      <c r="F56" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D56" s="51" t="s">
-        <v>115</v>
-      </c>
-      <c r="E56" s="73"/>
-      <c r="F56" s="55"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="66"/>
+      <c r="G56" s="103"/>
+      <c r="H56" s="50"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -3597,21 +3542,19 @@
       <c r="Z56" s="4"/>
       <c r="AA56" s="4"/>
     </row>
-    <row r="57" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A57" s="84"/>
-      <c r="B57" s="51" t="s">
-        <v>116</v>
+    <row r="57" spans="1:27" ht="18" customHeight="1">
+      <c r="A57" s="127"/>
+      <c r="B57" s="128"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="119" t="s">
+        <v>97</v>
       </c>
-      <c r="C57" s="67" t="s">
-        <v>156</v>
+      <c r="E57" s="129"/>
+      <c r="F57" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D57" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="E57" s="73"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="61"/>
-      <c r="H57" s="66"/>
+      <c r="G57" s="103"/>
+      <c r="H57" s="50"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -3632,21 +3575,19 @@
       <c r="Z57" s="4"/>
       <c r="AA57" s="4"/>
     </row>
-    <row r="58" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A58" s="84"/>
-      <c r="B58" s="51" t="s">
-        <v>144</v>
+    <row r="58" spans="1:27" ht="18.75" customHeight="1">
+      <c r="A58" s="127"/>
+      <c r="B58" s="128"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="119" t="s">
+        <v>98</v>
       </c>
-      <c r="C58" s="67" t="s">
-        <v>157</v>
+      <c r="E58" s="129"/>
+      <c r="F58" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D58" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="E58" s="73"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="61"/>
-      <c r="H58" s="66"/>
+      <c r="G58" s="103"/>
+      <c r="H58" s="50"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -3667,21 +3608,19 @@
       <c r="Z58" s="4"/>
       <c r="AA58" s="4"/>
     </row>
-    <row r="59" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A59" s="84"/>
-      <c r="B59" s="51" t="s">
-        <v>118</v>
+    <row r="59" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A59" s="127"/>
+      <c r="B59" s="128"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="119" t="s">
+        <v>99</v>
       </c>
-      <c r="C59" s="68" t="s">
-        <v>158</v>
+      <c r="E59" s="129"/>
+      <c r="F59" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D59" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="E59" s="73"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="61"/>
-      <c r="H59" s="66"/>
+      <c r="G59" s="103"/>
+      <c r="H59" s="50"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -3702,21 +3641,19 @@
       <c r="Z59" s="4"/>
       <c r="AA59" s="4"/>
     </row>
-    <row r="60" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A60" s="84"/>
-      <c r="B60" s="51" t="s">
-        <v>119</v>
+    <row r="60" spans="1:27" ht="16.5" customHeight="1">
+      <c r="A60" s="127"/>
+      <c r="B60" s="128"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="119" t="s">
+        <v>100</v>
       </c>
-      <c r="C60" s="69" t="s">
-        <v>159</v>
+      <c r="E60" s="129"/>
+      <c r="F60" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D60" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="E60" s="73"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="61"/>
-      <c r="H60" s="66"/>
+      <c r="G60" s="103"/>
+      <c r="H60" s="50"/>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -3737,21 +3674,19 @@
       <c r="Z60" s="4"/>
       <c r="AA60" s="4"/>
     </row>
-    <row r="61" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A61" s="84"/>
-      <c r="B61" s="51" t="s">
-        <v>120</v>
+    <row r="61" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A61" s="127"/>
+      <c r="B61" s="128"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="119" t="s">
+        <v>101</v>
       </c>
-      <c r="C61" s="69" t="s">
-        <v>160</v>
+      <c r="E61" s="129"/>
+      <c r="F61" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D61" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="E61" s="73"/>
-      <c r="F61" s="55"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="66"/>
+      <c r="G61" s="103"/>
+      <c r="H61" s="50"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -3772,21 +3707,19 @@
       <c r="Z61" s="4"/>
       <c r="AA61" s="4"/>
     </row>
-    <row r="62" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A62" s="84"/>
-      <c r="B62" s="51" t="s">
-        <v>121</v>
+    <row r="62" spans="1:27" ht="18.75" customHeight="1">
+      <c r="A62" s="127"/>
+      <c r="B62" s="128"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="119" t="s">
+        <v>102</v>
       </c>
-      <c r="C62" s="69" t="s">
-        <v>161</v>
+      <c r="E62" s="129"/>
+      <c r="F62" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D62" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="E62" s="73"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="61"/>
-      <c r="H62" s="66"/>
+      <c r="G62" s="103"/>
+      <c r="H62" s="50"/>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -3807,21 +3740,19 @@
       <c r="Z62" s="4"/>
       <c r="AA62" s="4"/>
     </row>
-    <row r="63" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A63" s="84"/>
-      <c r="B63" s="51" t="s">
-        <v>145</v>
+    <row r="63" spans="1:27" ht="19.5" customHeight="1">
+      <c r="A63" s="127"/>
+      <c r="B63" s="128"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="119" t="s">
+        <v>103</v>
       </c>
-      <c r="C63" s="69" t="s">
-        <v>162</v>
+      <c r="E63" s="129"/>
+      <c r="F63" s="104" t="s">
+        <v>147</v>
       </c>
-      <c r="D63" s="51" t="s">
-        <v>122</v>
-      </c>
-      <c r="E63" s="73"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="61"/>
-      <c r="H63" s="66"/>
+      <c r="G63" s="125"/>
+      <c r="H63" s="113"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -3842,15 +3773,19 @@
       <c r="Z63" s="4"/>
       <c r="AA63" s="4"/>
     </row>
-    <row r="64" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A64" s="4"/>
-      <c r="B64" s="58"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="57"/>
-      <c r="F64" s="58"/>
-      <c r="G64" s="58"/>
-      <c r="H64" s="59"/>
+    <row r="64" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A64" s="127"/>
+      <c r="B64" s="128"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="119" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" s="114"/>
+      <c r="F64" s="104" t="s">
+        <v>147</v>
+      </c>
+      <c r="G64" s="126"/>
+      <c r="H64" s="115"/>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -3871,15 +3806,19 @@
       <c r="Z64" s="4"/>
       <c r="AA64" s="4"/>
     </row>
-    <row r="65" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A65" s="4"/>
-      <c r="B65" s="58"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="57"/>
-      <c r="F65" s="58"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="59"/>
+    <row r="65" spans="1:27" ht="18" customHeight="1">
+      <c r="A65" s="127"/>
+      <c r="B65" s="128"/>
+      <c r="C65" s="112"/>
+      <c r="D65" s="119" t="s">
+        <v>105</v>
+      </c>
+      <c r="E65" s="114"/>
+      <c r="F65" s="104" t="s">
+        <v>147</v>
+      </c>
+      <c r="G65" s="126"/>
+      <c r="H65" s="115"/>
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
@@ -3902,13 +3841,13 @@
     </row>
     <row r="66" spans="1:27" ht="14.25" customHeight="1">
       <c r="A66" s="4"/>
-      <c r="B66" s="58"/>
+      <c r="B66" s="47"/>
       <c r="C66" s="5"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="57"/>
-      <c r="F66" s="58"/>
-      <c r="G66" s="58"/>
-      <c r="H66" s="59"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="48"/>
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
@@ -3931,13 +3870,13 @@
     </row>
     <row r="67" spans="1:27" ht="14.25" customHeight="1">
       <c r="A67" s="4"/>
-      <c r="B67" s="58"/>
+      <c r="B67" s="47"/>
       <c r="C67" s="5"/>
-      <c r="D67" s="49"/>
-      <c r="E67" s="57"/>
-      <c r="F67" s="58"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="59"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="48"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
@@ -3960,13 +3899,13 @@
     </row>
     <row r="68" spans="1:27" ht="14.25" customHeight="1">
       <c r="A68" s="4"/>
-      <c r="B68" s="58"/>
+      <c r="B68" s="47"/>
       <c r="C68" s="5"/>
-      <c r="D68" s="49"/>
-      <c r="E68" s="57"/>
-      <c r="F68" s="58"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="59"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="48"/>
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
@@ -12295,15 +12234,37 @@
       <c r="H1000" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A47:A63"/>
+  <mergeCells count="30">
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="B50:B65"/>
+    <mergeCell ref="A50:A65"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A23:A36"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A15:A21"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="A7:A16"/>
-    <mergeCell ref="A17:A33"/>
-    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A7:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -12330,15 +12291,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="104"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -12360,14 +12321,14 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="95"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
       <c r="G2" s="12"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -12393,12 +12354,12 @@
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="95"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="68"/>
       <c r="F3" s="14" t="s">
         <v>10</v>
       </c>
@@ -12429,14 +12390,14 @@
       <c r="A4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="96" t="s">
+      <c r="B4" s="69"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="99" t="s">
+      <c r="G4" s="73" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="4"/>
@@ -12463,12 +12424,12 @@
       <c r="A5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="100"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="74"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -12493,12 +12454,12 @@
       <c r="A6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="100"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="74"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -12523,12 +12484,12 @@
       <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="100"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="74"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -12553,14 +12514,14 @@
       <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="98" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="99" t="s">
+      <c r="G8" s="73" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="4"/>
@@ -12587,12 +12548,12 @@
       <c r="A9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="100"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="74"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -12617,14 +12578,14 @@
       <c r="A10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="96" t="s">
+      <c r="B10" s="69"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="99" t="s">
+      <c r="G10" s="73" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="4"/>
@@ -12651,12 +12612,12 @@
       <c r="A11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="93"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="100"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="74"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -12681,12 +12642,12 @@
       <c r="A12" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="93"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="100"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="74"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -12711,12 +12672,12 @@
       <c r="A13" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="100"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="74"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -12741,14 +12702,14 @@
       <c r="A14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="95"/>
-      <c r="F14" s="98" t="s">
+      <c r="B14" s="69"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="99" t="s">
+      <c r="G14" s="73" t="s">
         <v>30</v>
       </c>
       <c r="I14" s="4"/>
@@ -12774,12 +12735,12 @@
       <c r="A15" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="93"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="97"/>
-      <c r="G15" s="100"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="74"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -12804,14 +12765,14 @@
       <c r="A16" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="93"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="96" t="s">
+      <c r="B16" s="69"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="99" t="s">
+      <c r="G16" s="73" t="s">
         <v>34</v>
       </c>
       <c r="H16" s="4"/>
@@ -12838,12 +12799,12 @@
       <c r="A17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="97"/>
-      <c r="G17" s="100"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="74"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -12868,14 +12829,14 @@
       <c r="A18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="94"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="98" t="s">
+      <c r="B18" s="69"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="99" t="s">
+      <c r="G18" s="73" t="s">
         <v>38</v>
       </c>
       <c r="H18" s="4"/>
@@ -12902,12 +12863,12 @@
       <c r="A19" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="93"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="100"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="74"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -12932,12 +12893,12 @@
       <c r="A20" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="93"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="97"/>
-      <c r="G20" s="100"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="74"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -12962,14 +12923,14 @@
       <c r="A21" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="96" t="s">
+      <c r="B21" s="69"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="99" t="s">
+      <c r="G21" s="73" t="s">
         <v>43</v>
       </c>
       <c r="I21" s="4"/>
@@ -12995,12 +12956,12 @@
       <c r="A22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="97"/>
-      <c r="G22" s="100"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="74"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -13025,14 +12986,14 @@
       <c r="A23" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="98" t="s">
+      <c r="B23" s="69"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="99" t="s">
+      <c r="G23" s="73" t="s">
         <v>47</v>
       </c>
       <c r="H23" s="4"/>
@@ -13059,12 +13020,12 @@
       <c r="A24" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="93"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="100"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="74"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -21791,30 +21752,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="F21:F22"/>
@@ -21831,6 +21768,30 @@
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="F18:F20"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -21871,36 +21832,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:111" ht="21.75" customHeight="1">
-      <c r="A1" s="108"/>
-      <c r="B1" s="109"/>
-      <c r="C1" s="113" t="s">
+      <c r="A1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="114" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="116"/>
-      <c r="U1" s="117" t="s">
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="118"/>
-      <c r="W1" s="118"/>
-      <c r="X1" s="119"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="87"/>
       <c r="Y1" s="19"/>
       <c r="Z1" s="19"/>
       <c r="AA1" s="19"/>
@@ -21990,8 +21951,8 @@
       <c r="DG1" s="20"/>
     </row>
     <row r="2" spans="1:111" ht="18.75" customHeight="1">
-      <c r="A2" s="109"/>
-      <c r="B2" s="109"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
       <c r="C2" s="21" t="s">
         <v>52</v>
       </c>
@@ -22013,25 +21974,25 @@
       <c r="I2" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="120" t="s">
+      <c r="J2" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="115"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="120" t="s">
+      <c r="K2" s="83"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="116"/>
-      <c r="O2" s="120" t="s">
+      <c r="N2" s="84"/>
+      <c r="O2" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="120" t="s">
+      <c r="P2" s="83"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="115"/>
-      <c r="T2" s="116"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="84"/>
       <c r="U2" s="23" t="s">
         <v>63</v>
       </c>
@@ -22133,7 +22094,7 @@
       <c r="DG2" s="26"/>
     </row>
     <row r="3" spans="1:111" ht="21" customHeight="1">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="78" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="27" t="s">
@@ -22148,21 +22109,21 @@
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
-      <c r="J3" s="121" t="s">
+      <c r="J3" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="122"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="124"/>
-      <c r="N3" s="123"/>
-      <c r="O3" s="121" t="s">
+      <c r="K3" s="90"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="P3" s="122"/>
-      <c r="Q3" s="123"/>
-      <c r="R3" s="121"/>
-      <c r="S3" s="122"/>
-      <c r="T3" s="122"/>
+      <c r="P3" s="90"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="90"/>
+      <c r="T3" s="90"/>
       <c r="U3" s="30"/>
       <c r="V3" s="30"/>
       <c r="W3" s="30"/>
@@ -22256,7 +22217,7 @@
       <c r="DG3" s="11"/>
     </row>
     <row r="4" spans="1:111" ht="21" customHeight="1">
-      <c r="A4" s="111"/>
+      <c r="A4" s="79"/>
       <c r="B4" s="31" t="s">
         <v>70</v>
       </c>
@@ -22271,19 +22232,19 @@
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="105" t="s">
+      <c r="J4" s="93"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="95"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="95"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="94"/>
-      <c r="T4" s="94"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
       <c r="U4" s="30"/>
       <c r="V4" s="30"/>
       <c r="W4" s="30"/>
@@ -22377,7 +22338,7 @@
       <c r="DG4" s="11"/>
     </row>
     <row r="5" spans="1:111" ht="21" customHeight="1">
-      <c r="A5" s="111"/>
+      <c r="A5" s="79"/>
       <c r="B5" s="31" t="s">
         <v>71</v>
       </c>
@@ -22390,19 +22351,19 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
       <c r="I5" s="34"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="105" t="s">
+      <c r="J5" s="93"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="N5" s="95"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="95"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="94"/>
-      <c r="T5" s="94"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
       <c r="U5" s="30"/>
       <c r="V5" s="30"/>
       <c r="W5" s="30"/>
@@ -22496,7 +22457,7 @@
       <c r="DG5" s="11"/>
     </row>
     <row r="6" spans="1:111" ht="21" customHeight="1">
-      <c r="A6" s="111"/>
+      <c r="A6" s="79"/>
       <c r="B6" s="31" t="s">
         <v>72</v>
       </c>
@@ -22509,19 +22470,19 @@
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="105" t="s">
+      <c r="J6" s="93"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="N6" s="95"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="95"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="94"/>
-      <c r="T6" s="94"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="93"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
       <c r="U6" s="30"/>
       <c r="V6" s="30"/>
       <c r="W6" s="30"/>
@@ -22615,7 +22576,7 @@
       <c r="DG6" s="11"/>
     </row>
     <row r="7" spans="1:111" ht="21" customHeight="1">
-      <c r="A7" s="111"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="31" t="s">
         <v>73</v>
       </c>
@@ -22628,19 +22589,19 @@
       </c>
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="105" t="s">
+      <c r="J7" s="93"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="N7" s="95"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="95"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="94"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="93"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
       <c r="U7" s="30"/>
       <c r="V7" s="30"/>
       <c r="W7" s="30"/>
@@ -22734,7 +22695,7 @@
       <c r="DG7" s="11"/>
     </row>
     <row r="8" spans="1:111" ht="21" customHeight="1">
-      <c r="A8" s="111"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="31" t="s">
         <v>74</v>
       </c>
@@ -22747,19 +22708,19 @@
         <v>69</v>
       </c>
       <c r="I8" s="34"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="105" t="s">
+      <c r="J8" s="93"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="95"/>
-      <c r="O8" s="107"/>
-      <c r="P8" s="94"/>
-      <c r="Q8" s="95"/>
-      <c r="R8" s="107"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="94"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="94"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="67"/>
       <c r="U8" s="30"/>
       <c r="V8" s="30"/>
       <c r="W8" s="30"/>
@@ -22853,7 +22814,7 @@
       <c r="DG8" s="11"/>
     </row>
     <row r="9" spans="1:111" ht="21" customHeight="1">
-      <c r="A9" s="112"/>
+      <c r="A9" s="80"/>
       <c r="B9" s="31" t="s">
         <v>75</v>
       </c>
@@ -22866,19 +22827,19 @@
       <c r="I9" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="106"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="95"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="95"/>
-      <c r="R9" s="105" t="s">
+      <c r="J9" s="93"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="S9" s="94"/>
-      <c r="T9" s="94"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="67"/>
       <c r="U9" s="30"/>
       <c r="V9" s="30"/>
       <c r="W9" s="30"/>
@@ -57086,6 +57047,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="C1:I1"/>
@@ -57102,27 +57084,6 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="R4:T4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>